<commit_message>
prepravak baze podataka i css
</commit_message>
<xml_diff>
--- a/app/database/projekt_useri.xlsx
+++ b/app/database/projekt_useri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Desktop\rp2_projekt\rp2_projekt\app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBECD105-902B-4628-AEA1-C2E94091837B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06369480-D464-4CB8-B34E-E95D8BD0AE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="194">
   <si>
     <t>id_usera</t>
   </si>
@@ -524,6 +524,84 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>id_hotela</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>Ivana1</t>
+  </si>
+  <si>
+    <t>Kiki1</t>
+  </si>
+  <si>
+    <t>Dorotea1</t>
+  </si>
+  <si>
+    <t>Ivana2</t>
+  </si>
+  <si>
+    <t>Kiki2</t>
+  </si>
+  <si>
+    <t>Dorotea2</t>
+  </si>
+  <si>
+    <t>Ivana3</t>
+  </si>
+  <si>
+    <t>Kiki3</t>
+  </si>
+  <si>
+    <t>Dorotea3</t>
+  </si>
+  <si>
+    <t>Ivana4</t>
+  </si>
+  <si>
+    <t>Kiki4</t>
+  </si>
+  <si>
+    <t>Dorotea4</t>
   </si>
 </sst>
 </file>
@@ -910,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -922,7 +1000,7 @@
     <col min="4" max="4" width="9.25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -947,8 +1025,11 @@
       <c r="H1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -973,8 +1054,11 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -999,8 +1083,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1025,8 +1112,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1051,8 +1141,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1077,8 +1170,11 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1103,8 +1199,11 @@
       <c r="H7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1129,8 +1228,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1155,8 +1257,11 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1181,8 +1286,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1207,8 +1315,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1233,8 +1344,11 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1259,8 +1373,11 @@
       <c r="H13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1285,8 +1402,11 @@
       <c r="H14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1311,8 +1431,11 @@
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1337,8 +1460,11 @@
       <c r="H16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1363,8 +1489,11 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1389,8 +1518,11 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1415,8 +1547,11 @@
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1441,8 +1576,11 @@
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1467,8 +1605,11 @@
       <c r="H21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1493,8 +1634,11 @@
       <c r="H22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1519,8 +1663,11 @@
       <c r="H23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -1545,8 +1692,11 @@
       <c r="H24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1571,8 +1721,11 @@
       <c r="H25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -1597,8 +1750,11 @@
       <c r="H26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1623,8 +1779,11 @@
       <c r="H27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1649,8 +1808,11 @@
       <c r="H28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -1675,8 +1837,11 @@
       <c r="H29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1701,8 +1866,11 @@
       <c r="H30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -1727,8 +1895,11 @@
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -1753,8 +1924,11 @@
       <c r="H32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -1779,8 +1953,11 @@
       <c r="H33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1805,8 +1982,11 @@
       <c r="H34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -1831,8 +2011,11 @@
       <c r="H35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -1857,8 +2040,11 @@
       <c r="H36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -1883,8 +2069,11 @@
       <c r="H37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -1909,8 +2098,11 @@
       <c r="H38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -1935,8 +2127,11 @@
       <c r="H39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -1961,8 +2156,11 @@
       <c r="H40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -1987,8 +2185,11 @@
       <c r="H41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I41">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>103</v>
       </c>
@@ -2013,8 +2214,11 @@
       <c r="H42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I42">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -2039,8 +2243,11 @@
       <c r="H43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I43">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>108</v>
       </c>
@@ -2065,8 +2272,11 @@
       <c r="H44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>110</v>
       </c>
@@ -2091,8 +2301,11 @@
       <c r="H45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -2117,8 +2330,11 @@
       <c r="H46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I46">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>115</v>
       </c>
@@ -2143,8 +2359,11 @@
       <c r="H47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I47">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>118</v>
       </c>
@@ -2169,8 +2388,11 @@
       <c r="H48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>121</v>
       </c>
@@ -2195,8 +2417,11 @@
       <c r="H49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I49">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -2221,8 +2446,11 @@
       <c r="H50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>126</v>
       </c>
@@ -2247,8 +2475,11 @@
       <c r="H51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I51">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>128</v>
       </c>
@@ -2273,8 +2504,11 @@
       <c r="H52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I52">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>130</v>
       </c>
@@ -2299,8 +2533,11 @@
       <c r="H53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -2325,8 +2562,11 @@
       <c r="H54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I54">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -2351,8 +2591,11 @@
       <c r="H55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I55">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>136</v>
       </c>
@@ -2377,8 +2620,11 @@
       <c r="H56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I56">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>150</v>
       </c>
@@ -2403,8 +2649,11 @@
       <c r="H57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I57">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>151</v>
       </c>
@@ -2429,8 +2678,11 @@
       <c r="H58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I58">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>152</v>
       </c>
@@ -2454,6 +2706,357 @@
       </c>
       <c r="H59">
         <v>1</v>
+      </c>
+      <c r="I59">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60">
+        <v>181</v>
+      </c>
+      <c r="F60" t="s">
+        <v>166</v>
+      </c>
+      <c r="G60" t="s">
+        <v>167</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E61">
+        <v>182</v>
+      </c>
+      <c r="F61" t="s">
+        <v>166</v>
+      </c>
+      <c r="G61" t="s">
+        <v>167</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" t="s">
+        <v>184</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E62">
+        <v>183</v>
+      </c>
+      <c r="F62" t="s">
+        <v>166</v>
+      </c>
+      <c r="G62" t="s">
+        <v>167</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B63" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E63">
+        <v>184</v>
+      </c>
+      <c r="F63" t="s">
+        <v>166</v>
+      </c>
+      <c r="G63" t="s">
+        <v>167</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E64">
+        <v>185</v>
+      </c>
+      <c r="F64" t="s">
+        <v>166</v>
+      </c>
+      <c r="G64" t="s">
+        <v>167</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E65">
+        <v>186</v>
+      </c>
+      <c r="F65" t="s">
+        <v>166</v>
+      </c>
+      <c r="G65" t="s">
+        <v>167</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B66" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E66">
+        <v>187</v>
+      </c>
+      <c r="F66" t="s">
+        <v>166</v>
+      </c>
+      <c r="G66" t="s">
+        <v>167</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>177</v>
+      </c>
+      <c r="B67" t="s">
+        <v>189</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67">
+        <v>188</v>
+      </c>
+      <c r="F67" t="s">
+        <v>166</v>
+      </c>
+      <c r="G67" t="s">
+        <v>167</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>178</v>
+      </c>
+      <c r="B68" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E68">
+        <v>189</v>
+      </c>
+      <c r="F68" t="s">
+        <v>166</v>
+      </c>
+      <c r="G68" t="s">
+        <v>167</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>179</v>
+      </c>
+      <c r="B69" t="s">
+        <v>191</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E69">
+        <v>190</v>
+      </c>
+      <c r="F69" t="s">
+        <v>166</v>
+      </c>
+      <c r="G69" t="s">
+        <v>167</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>180</v>
+      </c>
+      <c r="B70" t="s">
+        <v>192</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E70">
+        <v>191</v>
+      </c>
+      <c r="F70" t="s">
+        <v>166</v>
+      </c>
+      <c r="G70" t="s">
+        <v>167</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>181</v>
+      </c>
+      <c r="B71" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71">
+        <v>192</v>
+      </c>
+      <c r="F71" t="s">
+        <v>166</v>
+      </c>
+      <c r="G71" t="s">
+        <v>167</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>